<commit_message>
added heurstics sheet and changed how heuristics are identified in experiment specifications.
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439426B2-B221-A448-B076-658956548797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A01920-D631-5E4D-B102-232A6532AADD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment-description" sheetId="2" r:id="rId1"/>
     <sheet name="experiment-specification" sheetId="1" r:id="rId2"/>
     <sheet name="run-description" sheetId="4" r:id="rId3"/>
     <sheet name="run-specification" sheetId="3" r:id="rId4"/>
+    <sheet name="heuristics" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>experiment_id</t>
   </si>
@@ -97,6 +98,18 @@
   </si>
   <si>
     <t>Run for daily report to LSH</t>
+  </si>
+  <si>
+    <t>heuristic_id</t>
+  </si>
+  <si>
+    <t>heuristic_1</t>
+  </si>
+  <si>
+    <t>heuristic_2</t>
+  </si>
+  <si>
+    <t>heuristic_3</t>
   </si>
 </sst>
 </file>
@@ -450,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -492,7 +505,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -524,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -535,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -546,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -711,4 +724,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16803A79-36E8-C242-9A3E-7A10F403054B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed name of heuristics sheet
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A01920-D631-5E4D-B102-232A6532AADD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FF968D-E708-774A-8271-C8E6506A0303}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="experiment-specification" sheetId="1" r:id="rId2"/>
     <sheet name="run-description" sheetId="4" r:id="rId3"/>
     <sheet name="run-specification" sheetId="3" r:id="rId4"/>
-    <sheet name="heuristics" sheetId="5" r:id="rId5"/>
+    <sheet name="heuristics-description" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -731,7 +731,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
added new run and new experiment
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FF968D-E708-774A-8271-C8E6506A0303}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619F96CB-F9C6-3D42-BE37-C22F0596810F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment-description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t>experiment_id</t>
   </si>
@@ -110,6 +110,24 @@
   </si>
   <si>
     <t>heuristic_3</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test run</t>
+  </si>
+  <si>
+    <t>Test experiment</t>
+  </si>
+  <si>
+    <t>extended</t>
+  </si>
+  <si>
+    <t>home-green</t>
+  </si>
+  <si>
+    <t>home-red</t>
   </si>
 </sst>
 </file>
@@ -461,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -495,6 +513,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -502,10 +531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -646,6 +675,129 @@
         <v>12</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -653,10 +805,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -687,6 +839,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -694,10 +857,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -721,6 +884,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -730,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16803A79-36E8-C242-9A3E-7A10F403054B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed name of sheets
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619F96CB-F9C6-3D42-BE37-C22F0596810F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681F4582-391A-5449-AFE4-3D47B8A2482E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
-    <sheet name="experiment-description" sheetId="2" r:id="rId1"/>
-    <sheet name="experiment-specification" sheetId="1" r:id="rId2"/>
-    <sheet name="run-description" sheetId="4" r:id="rId3"/>
-    <sheet name="run-specification" sheetId="3" r:id="rId4"/>
-    <sheet name="heuristics-description" sheetId="5" r:id="rId5"/>
+    <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
+    <sheet name="experiment_specification" sheetId="1" r:id="rId2"/>
+    <sheet name="run_description" sheetId="4" r:id="rId3"/>
+    <sheet name="run_specification" sheetId="3" r:id="rId4"/>
+    <sheet name="heuristics_description" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -481,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -909,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16803A79-36E8-C242-9A3E-7A10F403054B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
modification of the definition of max splitting variable
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681F4582-391A-5449-AFE4-3D47B8A2482E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5382B8-94E7-DF49-BAD7-79EBFA95ED8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="-17960" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="-33500" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
   <si>
     <t>experiment_id</t>
   </si>
@@ -128,13 +128,28 @@
   </si>
   <si>
     <t>home-red</t>
+  </si>
+  <si>
+    <t>inpatient_ward-green</t>
+  </si>
+  <si>
+    <t>inpatient_ward-red</t>
+  </si>
+  <si>
+    <t>intensive_care_unit-green</t>
+  </si>
+  <si>
+    <t>intensive_care_unit-red</t>
+  </si>
+  <si>
+    <t>age_three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -479,19 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -513,7 +528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -521,6 +536,28 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -531,20 +568,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A11" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -569,7 +606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -580,7 +617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -591,7 +628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -605,7 +642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -619,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -633,7 +670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -647,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -661,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -675,7 +712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -686,7 +723,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -700,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -714,7 +751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -728,7 +765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -742,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -750,51 +787,347 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C28" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
         <v>12</v>
       </c>
     </row>
@@ -811,13 +1144,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -828,7 +1161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -839,7 +1172,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -857,18 +1190,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -876,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -884,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -892,12 +1225,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -909,17 +1258,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16803A79-36E8-C242-9A3E-7A10F403054B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -927,7 +1276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -935,7 +1284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -943,7 +1292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
adjusted experiment template to allow for time dependent splitting variables
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F87DFD9-B23C-D24F-BC7A-788E27C50160}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792A5193-6B75-DA48-ADAA-C6F491A8070E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33500" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="41">
   <si>
     <t>experiment_id</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>age_three</t>
+  </si>
+  <si>
+    <t>time_independent</t>
+  </si>
+  <si>
+    <t>time_dependent</t>
+  </si>
+  <si>
+    <t>type_attribute</t>
   </si>
 </sst>
 </file>
@@ -568,20 +577,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A41"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,46 +599,49 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -636,69 +649,84 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -706,108 +734,129 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -815,13 +864,16 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -829,13 +881,16 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -843,13 +898,16 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -857,197 +915,230 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
         <v>15</v>
       </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
       <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
         <v>9</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
         <v>15</v>
       </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1055,27 +1146,33 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1083,13 +1180,16 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1097,13 +1197,16 @@
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1111,13 +1214,16 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1125,9 +1231,63 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
         <v>15</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E44" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bugs in using heuristics.
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792A5193-6B75-DA48-ADAA-C6F491A8070E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589B0F32-6E9D-8D44-A01D-42ED6C0E5F7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="3280" yWindow="-17480" windowWidth="25600" windowHeight="14700" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="43">
   <si>
     <t>experiment_id</t>
   </si>
@@ -152,13 +152,19 @@
   </si>
   <si>
     <t>type_attribute</t>
+  </si>
+  <si>
+    <t>length_of_stay_simple_two_weeks</t>
+  </si>
+  <si>
+    <t>length_of_stay_simple_week</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -509,13 +515,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -537,7 +543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -548,7 +554,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -559,7 +565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -580,10 +586,10 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
@@ -591,7 +597,7 @@
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -619,7 +625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -630,7 +636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -641,7 +647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -658,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -672,10 +678,10 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -692,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -709,7 +715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -723,10 +729,10 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -743,7 +749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>1</v>
       </c>
@@ -760,7 +766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>1</v>
       </c>
@@ -777,7 +783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>1</v>
       </c>
@@ -794,7 +800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>2</v>
       </c>
@@ -805,7 +811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>2</v>
       </c>
@@ -822,7 +828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>2</v>
       </c>
@@ -839,7 +845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -856,7 +862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
@@ -873,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2</v>
       </c>
@@ -890,7 +896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2</v>
       </c>
@@ -907,7 +913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2</v>
       </c>
@@ -924,7 +930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2</v>
       </c>
@@ -941,7 +947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2</v>
       </c>
@@ -958,7 +964,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>2</v>
       </c>
@@ -975,7 +981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>3</v>
       </c>
@@ -986,7 +992,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>3</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1008,7 +1014,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1059,7 +1065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1110,7 +1116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>4</v>
       </c>
@@ -1172,7 +1178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>4</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>4</v>
       </c>
@@ -1304,13 +1310,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1321,7 +1327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1332,7 +1338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1356,12 +1362,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1369,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1377,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1385,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1422,13 +1428,13 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1436,7 +1442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1452,7 +1458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
changes to experiment template, run evaluation and execute_run bash file in light of recent changes
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589B0F32-6E9D-8D44-A01D-42ED6C0E5F7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED806CA5-29C6-1B41-9394-A9B171021418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="-17480" windowWidth="25600" windowHeight="14700" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="43">
   <si>
     <t>experiment_id</t>
   </si>
@@ -142,9 +142,6 @@
     <t>intensive_care_unit-red</t>
   </si>
   <si>
-    <t>age_three</t>
-  </si>
-  <si>
     <t>time_independent</t>
   </si>
   <si>
@@ -158,13 +155,16 @@
   </si>
   <si>
     <t>length_of_stay_simple_week</t>
+  </si>
+  <si>
+    <t>length_of_stay_simple_three_days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -509,19 +509,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -543,7 +543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -551,10 +551,10 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -565,7 +565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -573,6 +573,28 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -583,21 +605,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A11" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -614,7 +636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -625,7 +647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -636,7 +658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -647,7 +669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -655,7 +677,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -664,7 +686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -672,16 +694,16 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -689,7 +711,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -698,7 +720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -706,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -715,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -723,16 +745,16 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -740,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -749,7 +771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -757,7 +779,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -766,7 +788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -774,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -783,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -791,7 +813,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -800,7 +822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -811,92 +833,80 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -904,21 +914,21 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
@@ -930,24 +940,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -955,21 +965,21 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -981,18 +991,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1000,10 +1016,10 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1011,35 +1027,29 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -1048,7 +1058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1059,13 +1069,13 @@
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1073,16 +1083,16 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1090,63 +1100,69 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
-        <v>4</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" t="s">
-        <v>31</v>
-      </c>
       <c r="E35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -1155,98 +1171,80 @@
         <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1257,43 +1255,806 @@
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" t="s">
         <v>15</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D59" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>37</v>
+      </c>
+      <c r="D61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>37</v>
+      </c>
+      <c r="D68" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>5</v>
+      </c>
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" t="s">
+        <v>36</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>5</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>37</v>
+      </c>
+      <c r="D70" t="s">
+        <v>36</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" t="s">
+        <v>31</v>
+      </c>
+      <c r="E74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" t="s">
+        <v>31</v>
+      </c>
+      <c r="E75" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" t="s">
+        <v>32</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>32</v>
+      </c>
+      <c r="E78" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" t="s">
+        <v>32</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" t="s">
+        <v>37</v>
+      </c>
+      <c r="D80" t="s">
+        <v>33</v>
+      </c>
+      <c r="E80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" t="s">
+        <v>33</v>
+      </c>
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" t="s">
+        <v>37</v>
+      </c>
+      <c r="D82" t="s">
+        <v>33</v>
+      </c>
+      <c r="E82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" t="s">
+        <v>37</v>
+      </c>
+      <c r="D83" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" t="s">
+        <v>37</v>
+      </c>
+      <c r="D85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="s">
+        <v>37</v>
+      </c>
+      <c r="D86" t="s">
+        <v>35</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
+        <v>38</v>
+      </c>
+      <c r="D87" t="s">
+        <v>35</v>
+      </c>
+      <c r="E87" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>37</v>
+      </c>
+      <c r="D88" t="s">
+        <v>35</v>
+      </c>
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>6</v>
+      </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" t="s">
+        <v>37</v>
+      </c>
+      <c r="D89" t="s">
+        <v>36</v>
+      </c>
+      <c r="E89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>6</v>
+      </c>
+      <c r="B90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" t="s">
+        <v>38</v>
+      </c>
+      <c r="D90" t="s">
+        <v>36</v>
+      </c>
+      <c r="E90" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>6</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" t="s">
+        <v>37</v>
+      </c>
+      <c r="D91" t="s">
+        <v>36</v>
+      </c>
+      <c r="E91" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1304,19 +2065,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1327,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1338,7 +2099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1346,6 +2107,17 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1356,18 +2128,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1375,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1383,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1391,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1399,7 +2171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1407,12 +2179,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1428,13 +2216,13 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1442,7 +2230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1450,7 +2238,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1458,7 +2246,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
adding point of diagnosis as splitting variable
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED806CA5-29C6-1B41-9394-A9B171021418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA878B2B-B169-6E46-B117-172D577DBFED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="-37840" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="47">
   <si>
     <t>experiment_id</t>
   </si>
@@ -154,10 +154,22 @@
     <t>length_of_stay_simple_two_weeks</t>
   </si>
   <si>
-    <t>length_of_stay_simple_week</t>
-  </si>
-  <si>
-    <t>length_of_stay_simple_three_days</t>
+    <t>priority comparison</t>
+  </si>
+  <si>
+    <t>Base case with two weeks time dependent splitting in home state</t>
+  </si>
+  <si>
+    <t>time_dependent_splitting_test</t>
+  </si>
+  <si>
+    <t>age_simple_point_of_diagnosis</t>
+  </si>
+  <si>
+    <t>point_of_diagnosis</t>
+  </si>
+  <si>
+    <t>point in diagnosis splitting test</t>
   </si>
 </sst>
 </file>
@@ -511,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -605,10 +617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,10 +653,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -652,10 +670,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -663,10 +687,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -680,7 +710,7 @@
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -697,7 +727,7 @@
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -714,10 +744,10 @@
         <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -731,7 +761,7 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -748,7 +778,7 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -765,7 +795,7 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -773,7 +803,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -782,7 +812,7 @@
         <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -790,7 +820,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -799,15 +829,15 @@
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -816,10 +846,10 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -827,10 +857,16 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -838,10 +874,16 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -849,10 +891,16 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -866,7 +914,7 @@
         <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -883,10 +931,10 @@
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -900,15 +948,15 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -917,7 +965,7 @@
         <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -925,7 +973,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -934,15 +982,15 @@
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -951,15 +999,15 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -968,15 +1016,15 @@
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -985,7 +1033,7 @@
         <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -993,7 +1041,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1002,7 +1050,7 @@
         <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -1013,10 +1061,16 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1024,10 +1078,16 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1035,15 +1095,21 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -1060,7 +1126,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -1077,7 +1143,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
@@ -1094,7 +1160,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -1106,12 +1172,12 @@
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -1123,12 +1189,12 @@
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -1140,12 +1206,12 @@
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -1162,7 +1228,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -1179,7 +1245,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
@@ -1196,7 +1262,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -1207,7 +1273,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
@@ -1218,7 +1284,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -1229,7 +1295,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -1238,7 +1304,7 @@
         <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1246,7 +1312,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -1255,15 +1321,15 @@
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E42" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
@@ -1272,7 +1338,7 @@
         <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1280,7 +1346,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
@@ -1289,7 +1355,7 @@
         <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1297,7 +1363,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -1306,15 +1372,15 @@
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E45" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
@@ -1323,15 +1389,15 @@
         <v>37</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -1340,7 +1406,7 @@
         <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -1348,7 +1414,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
         <v>6</v>
@@ -1357,7 +1423,7 @@
         <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1365,7 +1431,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -1374,7 +1440,7 @@
         <v>37</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -1385,10 +1451,16 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
+        <v>34</v>
       </c>
       <c r="E50" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1396,10 +1468,16 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1407,10 +1485,16 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" t="s">
+        <v>34</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1424,7 +1508,7 @@
         <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
@@ -1441,7 +1525,7 @@
         <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -1458,10 +1542,10 @@
         <v>37</v>
       </c>
       <c r="D55" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1475,7 +1559,7 @@
         <v>37</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E56" t="s">
         <v>10</v>
@@ -1492,7 +1576,7 @@
         <v>38</v>
       </c>
       <c r="D57" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -1509,66 +1593,48 @@
         <v>37</v>
       </c>
       <c r="D58" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E58" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" t="s">
-        <v>37</v>
-      </c>
-      <c r="D59" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" t="s">
-        <v>37</v>
-      </c>
-      <c r="D61" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -1577,7 +1643,7 @@
         <v>37</v>
       </c>
       <c r="D62" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -1585,7 +1651,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
@@ -1594,15 +1660,15 @@
         <v>38</v>
       </c>
       <c r="D63" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
@@ -1611,15 +1677,15 @@
         <v>37</v>
       </c>
       <c r="D64" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
@@ -1628,7 +1694,7 @@
         <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E65" t="s">
         <v>10</v>
@@ -1636,7 +1702,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -1645,7 +1711,7 @@
         <v>38</v>
       </c>
       <c r="D66" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E66" t="s">
         <v>12</v>
@@ -1653,7 +1719,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
@@ -1662,15 +1728,15 @@
         <v>37</v>
       </c>
       <c r="D67" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E67" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -1679,7 +1745,7 @@
         <v>37</v>
       </c>
       <c r="D68" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -1687,7 +1753,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
@@ -1696,7 +1762,7 @@
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E69" t="s">
         <v>12</v>
@@ -1704,7 +1770,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -1713,7 +1779,7 @@
         <v>37</v>
       </c>
       <c r="D70" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E70" t="s">
         <v>12</v>
@@ -1724,10 +1790,16 @@
         <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>37</v>
+      </c>
+      <c r="D71" t="s">
+        <v>34</v>
       </c>
       <c r="E71" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -1735,10 +1807,16 @@
         <v>6</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>34</v>
       </c>
       <c r="E72" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -1746,10 +1824,16 @@
         <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73" t="s">
+        <v>34</v>
       </c>
       <c r="E73" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -1763,7 +1847,7 @@
         <v>37</v>
       </c>
       <c r="D74" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E74" t="s">
         <v>10</v>
@@ -1780,10 +1864,10 @@
         <v>38</v>
       </c>
       <c r="D75" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E75" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -1797,10 +1881,10 @@
         <v>37</v>
       </c>
       <c r="D76" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E76" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -1814,7 +1898,7 @@
         <v>37</v>
       </c>
       <c r="D77" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -1831,10 +1915,10 @@
         <v>38</v>
       </c>
       <c r="D78" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E78" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -1848,213 +1932,9 @@
         <v>37</v>
       </c>
       <c r="D79" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>6</v>
-      </c>
-      <c r="B80" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" t="s">
-        <v>37</v>
-      </c>
-      <c r="D80" t="s">
-        <v>33</v>
-      </c>
-      <c r="E80" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>6</v>
-      </c>
-      <c r="B81" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" t="s">
-        <v>38</v>
-      </c>
-      <c r="D81" t="s">
-        <v>33</v>
-      </c>
-      <c r="E81" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>6</v>
-      </c>
-      <c r="B82" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82" t="s">
-        <v>37</v>
-      </c>
-      <c r="D82" t="s">
-        <v>33</v>
-      </c>
-      <c r="E82" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>6</v>
-      </c>
-      <c r="B83" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" t="s">
-        <v>37</v>
-      </c>
-      <c r="D83" t="s">
-        <v>34</v>
-      </c>
-      <c r="E83" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>6</v>
-      </c>
-      <c r="B84" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" t="s">
-        <v>38</v>
-      </c>
-      <c r="D84" t="s">
-        <v>34</v>
-      </c>
-      <c r="E84" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>6</v>
-      </c>
-      <c r="B85" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" t="s">
-        <v>37</v>
-      </c>
-      <c r="D85" t="s">
-        <v>34</v>
-      </c>
-      <c r="E85" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>6</v>
-      </c>
-      <c r="B86" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D86" t="s">
-        <v>35</v>
-      </c>
-      <c r="E86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>6</v>
-      </c>
-      <c r="B87" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" t="s">
-        <v>38</v>
-      </c>
-      <c r="D87" t="s">
-        <v>35</v>
-      </c>
-      <c r="E87" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>6</v>
-      </c>
-      <c r="B88" t="s">
-        <v>9</v>
-      </c>
-      <c r="C88" t="s">
-        <v>37</v>
-      </c>
-      <c r="D88" t="s">
-        <v>35</v>
-      </c>
-      <c r="E88" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>6</v>
-      </c>
-      <c r="B89" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" t="s">
-        <v>37</v>
-      </c>
-      <c r="D89" t="s">
-        <v>36</v>
-      </c>
-      <c r="E89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>6</v>
-      </c>
-      <c r="B90" t="s">
-        <v>6</v>
-      </c>
-      <c r="C90" t="s">
-        <v>38</v>
-      </c>
-      <c r="D90" t="s">
-        <v>36</v>
-      </c>
-      <c r="E90" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>6</v>
-      </c>
-      <c r="B91" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" t="s">
-        <v>37</v>
-      </c>
-      <c r="D91" t="s">
-        <v>36</v>
-      </c>
-      <c r="E91" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2065,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2104,7 +1984,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -2119,6 +1999,28 @@
       </c>
       <c r="C4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2128,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,10 +2083,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2192,15 +2094,47 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="B8">
-        <v>6</v>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes ahead of Sölvi
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED806CA5-29C6-1B41-9394-A9B171021418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA075ACF-C6B3-834D-8E49-0E1FFD6787B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="1880" yWindow="-18420" windowWidth="25600" windowHeight="14640" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,17 +511,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -543,7 +543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -554,7 +554,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -565,7 +565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -576,7 +576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -587,7 +587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -607,11 +607,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
@@ -619,7 +619,7 @@
     <col min="5" max="5" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -647,7 +647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -658,7 +658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -669,7 +669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -686,7 +686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -703,7 +703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -720,7 +720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -737,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -754,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -771,7 +771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>1</v>
       </c>
@@ -788,7 +788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>1</v>
       </c>
@@ -805,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>1</v>
       </c>
@@ -822,7 +822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>2</v>
       </c>
@@ -833,7 +833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>2</v>
       </c>
@@ -844,7 +844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>2</v>
       </c>
@@ -855,7 +855,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -872,7 +872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
@@ -889,7 +889,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2</v>
       </c>
@@ -906,7 +906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2</v>
       </c>
@@ -923,7 +923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2</v>
       </c>
@@ -940,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2</v>
       </c>
@@ -957,7 +957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2</v>
       </c>
@@ -974,7 +974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>2</v>
       </c>
@@ -991,7 +991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>4</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>4</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>4</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>4</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>4</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>4</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>4</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>5</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>5</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>5</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>5</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>5</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>5</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>5</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>5</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>5</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>5</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>5</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>5</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>5</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>5</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>5</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>5</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>5</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>5</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>5</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>5</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>6</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>6</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>6</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>6</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>6</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>6</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>6</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>6</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>6</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>6</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>6</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>6</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>6</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>6</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>6</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>6</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>6</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>6</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>6</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>6</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>6</v>
       </c>
@@ -2071,13 +2071,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2128,18 +2128,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2187,19 +2187,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
         <v>6</v>
       </c>
     </row>
@@ -2216,13 +2232,13 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2230,7 +2246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2238,7 +2254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2246,7 +2262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Bug fix + added new heuristic + experiments.
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D0737-D8C7-BA42-AF26-38A1C328505B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F83002-010C-8B4A-845F-946F5E6D1126}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1700" yWindow="-19060" windowWidth="25600" windowHeight="14660" activeTab="4" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="5480" yWindow="-18780" windowWidth="25600" windowHeight="14660" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="49">
   <si>
     <t>experiment_id</t>
   </si>
@@ -161,6 +161,21 @@
   </si>
   <si>
     <t>LOS driven: 4 + point of diag splitting of length of stay in Inpatient Ward</t>
+  </si>
+  <si>
+    <t>Comparing Base and CA</t>
+  </si>
+  <si>
+    <t>hospital_less_than_14_days: If home and worst state is home and next state is not recovered length of stay has to be less than 14 days.</t>
+  </si>
+  <si>
+    <t>Transition driven: 1 + hospital_less_than_14_days heuristic</t>
+  </si>
+  <si>
+    <t>1;2;3;5</t>
+  </si>
+  <si>
+    <t>Comparing aggressive transition and los driven base models</t>
   </si>
 </sst>
 </file>
@@ -512,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -610,43 +625,57 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>1001</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>1003</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -657,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -949,10 +978,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>1001</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -966,10 +995,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>1001</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -978,15 +1007,15 @@
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>1001</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1003,7 +1032,7 @@
         <v>1001</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -1012,7 +1041,7 @@
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1020,7 +1049,7 @@
         <v>1001</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -1029,7 +1058,7 @@
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1037,7 +1066,7 @@
         <v>1001</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -1051,10 +1080,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -1063,15 +1092,15 @@
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -1080,15 +1109,15 @@
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -1105,7 +1134,7 @@
         <v>1002</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -1114,7 +1143,7 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1122,7 +1151,7 @@
         <v>1002</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -1131,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1139,7 +1168,7 @@
         <v>1002</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1153,27 +1182,27 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -1182,15 +1211,15 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -1207,16 +1236,16 @@
         <v>1003</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1224,7 +1253,7 @@
         <v>1003</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -1233,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1241,15 +1270,66 @@
         <v>1003</v>
       </c>
       <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>1003</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>1003</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>1003</v>
+      </c>
+      <c r="B37" t="s">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1260,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1311,6 +1391,22 @@
         <v>42</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1318,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1417,6 +1513,54 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1424,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16803A79-36E8-C242-9A3E-7A10F403054B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1476,6 +1620,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
experiment template new experiments
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F83002-010C-8B4A-845F-946F5E6D1126}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8000B4-9DEB-7D4C-81B0-D58C1D5D45FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="-18780" windowWidth="25600" windowHeight="14660" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="-36680" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="53">
   <si>
     <t>experiment_id</t>
   </si>
@@ -176,13 +176,25 @@
   </si>
   <si>
     <t>Comparing aggressive transition and los driven base models</t>
+  </si>
+  <si>
+    <t>LOS driven:3 + treatment constraints splitting of transitions  in Inpatient Ward</t>
+  </si>
+  <si>
+    <t>LOS driven:7 + treatment_constraints splitting in length of stay in Inpatient Ward</t>
+  </si>
+  <si>
+    <t>age_simple_intensive_care_unit_restriction</t>
+  </si>
+  <si>
+    <t>Testing treatment constraint splitting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -527,19 +539,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="83.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -567,7 +579,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -581,7 +593,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -595,7 +607,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -609,7 +621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -623,7 +635,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -637,45 +649,73 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1001</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1002</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1002</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1003</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -686,25 +726,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="4" max="5" width="38.1640625" customWidth="1"/>
     <col min="6" max="6" width="31.1640625" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -738,7 +777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -755,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -772,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -789,7 +828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -806,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -823,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -840,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -857,7 +896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -874,7 +913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -891,7 +930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -908,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -925,7 +964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -942,7 +981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -959,7 +998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -976,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -993,7 +1032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1010,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1027,111 +1066,111 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>1001</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
-        <v>1001</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
-        <v>1001</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>1001</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>1001</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>1001</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
-        <v>1002</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
@@ -1146,9 +1185,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
@@ -1163,9 +1202,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
@@ -1180,9 +1219,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -1197,9 +1236,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -1214,9 +1253,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B31" t="s">
         <v>19</v>
@@ -1231,15 +1270,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -1248,9 +1287,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
@@ -1265,9 +1304,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
@@ -1282,9 +1321,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -1299,9 +1338,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
@@ -1316,9 +1355,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
@@ -1330,6 +1369,108 @@
         <v>4</v>
       </c>
       <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1003</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1003</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1003</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1003</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1003</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1003</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1340,18 +1481,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1359,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1367,7 +1508,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1375,7 +1516,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1383,7 +1524,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1391,7 +1532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1399,12 +1540,20 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1414,18 +1563,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1433,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1441,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1449,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1457,7 +1606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1465,7 +1614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1473,7 +1622,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1481,7 +1630,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1489,7 +1638,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1497,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1505,7 +1654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1513,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1521,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1529,7 +1678,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1537,7 +1686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1545,7 +1694,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1553,12 +1702,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17">
         <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1574,13 +1747,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1588,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1596,7 +1769,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1604,7 +1777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1612,7 +1785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1620,7 +1793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
bug fix length of stay for treatment constraints
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8000B4-9DEB-7D4C-81B0-D58C1D5D45FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB28E9AC-634F-8245-86F3-CA55F18E69CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36680" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="-36460" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -541,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1565,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added -r to bash + small fixes
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB28E9AC-634F-8245-86F3-CA55F18E69CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17FD34D-99A1-EC42-953C-F943F779FEFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36460" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="4240" yWindow="-18920" windowWidth="25600" windowHeight="14720" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="54">
   <si>
     <t>experiment_id</t>
   </si>
@@ -188,13 +188,16 @@
   </si>
   <si>
     <t>Testing treatment constraint splitting</t>
+  </si>
+  <si>
+    <t>LOS driven:3+treatment constraints splitting of length of stay in Inpatient Ward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -539,19 +542,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="83.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +568,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -579,7 +582,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -593,7 +596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -607,7 +610,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -621,7 +624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -635,7 +638,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -649,7 +652,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -663,12 +666,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -677,45 +680,59 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17" customHeight="1">
       <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
         <v>1001</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1002</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>1003</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -726,13 +743,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
@@ -743,7 +760,7 @@
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -777,7 +794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -794,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -811,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>2</v>
       </c>
@@ -828,7 +845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -845,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>2</v>
       </c>
@@ -862,7 +879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>3</v>
       </c>
@@ -879,7 +896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>3</v>
       </c>
@@ -896,7 +913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>3</v>
       </c>
@@ -913,7 +930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>4</v>
       </c>
@@ -930,7 +947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>4</v>
       </c>
@@ -947,7 +964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>4</v>
       </c>
@@ -964,7 +981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>5</v>
       </c>
@@ -981,7 +998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>5</v>
       </c>
@@ -998,7 +1015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1015,7 +1032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1032,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1049,7 +1066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1066,7 +1083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1083,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1100,7 +1117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1117,7 +1134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1134,7 +1151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1145,13 +1162,13 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1168,15 +1185,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
-        <v>1001</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -1185,29 +1202,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
-        <v>1001</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
-        <v>1001</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1219,12 +1236,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>1001</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -1233,15 +1250,15 @@
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>1001</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -1250,67 +1267,67 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>1001</v>
       </c>
       <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>1001</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>1001</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>1001</v>
+      </c>
+      <c r="B34" t="s">
         <v>19</v>
       </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>1002</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>1002</v>
-      </c>
-      <c r="B33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>1002</v>
-      </c>
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
@@ -1321,12 +1338,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>1002</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
@@ -1335,15 +1352,15 @@
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>1002</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -1352,67 +1369,67 @@
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>1002</v>
       </c>
       <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>1002</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>1002</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>1002</v>
+      </c>
+      <c r="B40" t="s">
         <v>19</v>
       </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>1003</v>
-      </c>
-      <c r="B38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1003</v>
-      </c>
-      <c r="B39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1003</v>
-      </c>
-      <c r="B40" t="s">
-        <v>16</v>
-      </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
@@ -1423,29 +1440,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>1003</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>1003</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -1454,23 +1471,74 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>1003</v>
       </c>
       <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>1003</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>1003</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>1003</v>
+      </c>
+      <c r="B46" t="s">
         <v>19</v>
       </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1487,12 +1555,12 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1500,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1508,7 +1576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1516,7 +1584,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1524,7 +1592,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1532,7 +1600,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1540,7 +1608,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1548,7 +1616,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1563,18 +1631,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1582,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1590,7 +1658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1598,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1606,7 +1674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1614,7 +1682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1622,7 +1690,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1630,7 +1698,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1638,7 +1706,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1646,7 +1714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1654,7 +1722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1662,7 +1730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1670,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1678,7 +1746,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1686,7 +1754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1694,7 +1762,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1702,7 +1770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1710,7 +1778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1718,7 +1786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1726,12 +1794,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>7</v>
       </c>
       <c r="B20">
         <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1747,13 +1823,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1761,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1769,7 +1845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1777,7 +1853,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1785,7 +1861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1793,7 +1869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Changed distribution back to lognormal + max length to 28 days.
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17FD34D-99A1-EC42-953C-F943F779FEFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC74E0-0168-A54D-B774-D2AD3D9D8A02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="-18920" windowWidth="25600" windowHeight="14720" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="4240" yWindow="-18920" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1029,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1633,7 +1633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added specification for the Ferguson model
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B0844C-7F8F-1142-BD28-D8CF2B05D0CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EF40B3-B700-2348-B7B4-F66BB6FC8409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="-18920" windowWidth="25600" windowHeight="14720" activeTab="2" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="58">
   <si>
     <t>experiment_id</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>LOS driven:3+treatment constraints splitting of length of stay in Inpatient Ward</t>
+  </si>
+  <si>
+    <t>ferguson_state_worst: Patients who leave ICU recover after one day in ward.</t>
+  </si>
+  <si>
+    <t>Ferguson model</t>
+  </si>
+  <si>
+    <t>4;6</t>
+  </si>
+  <si>
+    <t>Compare Ferguson model</t>
   </si>
 </sst>
 </file>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -694,45 +706,59 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="17" customHeight="1">
       <c r="A11">
-        <v>1001</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>1003</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -743,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A8" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1238,50 +1264,50 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>1001</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>1001</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>1001</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -1292,7 +1318,7 @@
         <v>1001</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1301,7 +1327,7 @@
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1309,7 +1335,7 @@
         <v>1001</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -1318,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1326,7 +1352,7 @@
         <v>1001</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -1340,10 +1366,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
@@ -1352,15 +1378,15 @@
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -1369,15 +1395,15 @@
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1394,7 +1420,7 @@
         <v>1002</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -1403,7 +1429,7 @@
         <v>4</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1411,7 +1437,7 @@
         <v>1002</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -1420,7 +1446,7 @@
         <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1428,7 +1454,7 @@
         <v>1002</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
@@ -1442,27 +1468,27 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -1471,15 +1497,15 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -1496,16 +1522,16 @@
         <v>1003</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1513,7 +1539,7 @@
         <v>1003</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -1522,7 +1548,7 @@
         <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1530,15 +1556,66 @@
         <v>1003</v>
       </c>
       <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>1003</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>1003</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>1003</v>
+      </c>
+      <c r="B49" t="s">
         <v>19</v>
       </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1549,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1624,6 +1701,14 @@
         <v>52</v>
       </c>
     </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1631,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1810,6 +1895,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1817,10 +1910,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16803A79-36E8-C242-9A3E-7A10F403054B}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1877,6 +1970,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support for priors
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EF40B3-B700-2348-B7B4-F66BB6FC8409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054EA5EC-2FF2-6342-AC73-EDC5A187815E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="63">
   <si>
     <t>experiment_id</t>
   </si>
@@ -196,20 +196,35 @@
     <t>ferguson_state_worst: Patients who leave ICU recover after one day in ward.</t>
   </si>
   <si>
-    <t>Ferguson model</t>
-  </si>
-  <si>
     <t>4;6</t>
   </si>
   <si>
     <t>Compare Ferguson model</t>
+  </si>
+  <si>
+    <t>ferguson</t>
+  </si>
+  <si>
+    <t>age_official</t>
+  </si>
+  <si>
+    <t>prior_transition</t>
+  </si>
+  <si>
+    <t>prior_los</t>
+  </si>
+  <si>
+    <t>Ferguson Wuhan model</t>
+  </si>
+  <si>
+    <t>wuhan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,19 +569,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="83.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,8 +595,14 @@
       <c r="D1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -593,8 +615,14 @@
       <c r="D2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -607,8 +635,14 @@
       <c r="D3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -621,8 +655,14 @@
       <c r="D4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -635,8 +675,14 @@
       <c r="D5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -649,8 +695,14 @@
       <c r="D6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -663,8 +715,14 @@
       <c r="D7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -677,8 +735,14 @@
       <c r="D8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -691,8 +755,14 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" customHeight="1">
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -705,22 +775,34 @@
       <c r="D10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" customHeight="1">
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
         <v>55</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1001</v>
       </c>
@@ -733,8 +815,14 @@
       <c r="D12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1002</v>
       </c>
@@ -747,8 +835,14 @@
       <c r="D13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1003</v>
       </c>
@@ -760,6 +854,12 @@
       </c>
       <c r="D14" t="s">
         <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -771,11 +871,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A6" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
@@ -786,7 +886,7 @@
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -803,7 +903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -820,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -837,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -854,7 +954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -871,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -888,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -905,7 +1005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -922,7 +1022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -939,7 +1039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -956,7 +1056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -973,7 +1073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -990,7 +1090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1007,7 +1107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1024,7 +1124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1041,7 +1141,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1058,7 +1158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1075,7 +1175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1092,7 +1192,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1109,7 +1209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1126,7 +1226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1143,7 +1243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1160,7 +1260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1177,7 +1277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1194,7 +1294,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1211,7 +1311,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1228,7 +1328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1245,7 +1345,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1262,7 +1362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1270,16 +1370,16 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1287,16 +1387,16 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1313,7 +1413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1001</v>
       </c>
@@ -1330,7 +1430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1001</v>
       </c>
@@ -1347,7 +1447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1001</v>
       </c>
@@ -1364,7 +1464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1001</v>
       </c>
@@ -1381,7 +1481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1001</v>
       </c>
@@ -1398,7 +1498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1001</v>
       </c>
@@ -1415,7 +1515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1002</v>
       </c>
@@ -1432,7 +1532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1002</v>
       </c>
@@ -1449,7 +1549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1002</v>
       </c>
@@ -1466,7 +1566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1002</v>
       </c>
@@ -1483,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1002</v>
       </c>
@@ -1500,7 +1600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1002</v>
       </c>
@@ -1517,7 +1617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1003</v>
       </c>
@@ -1534,7 +1634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1003</v>
       </c>
@@ -1551,7 +1651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1003</v>
       </c>
@@ -1568,7 +1668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1003</v>
       </c>
@@ -1585,7 +1685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1003</v>
       </c>
@@ -1602,7 +1702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1003</v>
       </c>
@@ -1632,12 +1732,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1645,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1653,7 +1753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1661,7 +1761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1669,7 +1769,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1677,7 +1777,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1685,7 +1785,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1693,7 +1793,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1701,12 +1801,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1718,16 +1818,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1735,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1743,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1751,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1759,7 +1859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1767,7 +1867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1775,7 +1875,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1783,7 +1883,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1791,7 +1891,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1799,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1807,7 +1907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1815,7 +1915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1823,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1831,7 +1931,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1839,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1847,7 +1947,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1855,7 +1955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1863,7 +1963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1871,7 +1971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1879,7 +1979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1887,7 +1987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1895,7 +1995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1916,13 +2016,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1930,7 +2030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1938,7 +2038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1946,7 +2046,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1954,7 +2054,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1962,7 +2062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1970,7 +2070,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added priors and experiment specification for iceland ferguson model.
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054EA5EC-2FF2-6342-AC73-EDC5A187815E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA148A1-34AB-F24F-A7FC-0B7CCA1B3AF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="67">
   <si>
     <t>experiment_id</t>
   </si>
@@ -199,9 +199,6 @@
     <t>4;6</t>
   </si>
   <si>
-    <t>Compare Ferguson model</t>
-  </si>
-  <si>
     <t>ferguson</t>
   </si>
   <si>
@@ -218,13 +215,28 @@
   </si>
   <si>
     <t>wuhan</t>
+  </si>
+  <si>
+    <t>Ferguson Iceland model</t>
+  </si>
+  <si>
+    <t>iceland</t>
+  </si>
+  <si>
+    <t>Ferguson mixed model</t>
+  </si>
+  <si>
+    <t>length_of_stay_simple_week</t>
+  </si>
+  <si>
+    <t>Compare Ferguson models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -569,20 +581,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="83.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,13 +608,13 @@
         <v>30</v>
       </c>
       <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -622,7 +634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -642,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -662,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -682,7 +694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -702,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -722,7 +734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -742,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -762,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17" customHeight="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -782,83 +794,123 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17" customHeight="1">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
       </c>
       <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" customHeight="1">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="F11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" customHeight="1">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
         <v>1001</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1002</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1003</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>1002</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>1003</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -869,13 +921,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A15" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
@@ -886,7 +938,7 @@
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -903,7 +955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -920,7 +972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -937,7 +989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -954,7 +1006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>2</v>
       </c>
@@ -971,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -988,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1005,7 +1057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1022,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1039,7 +1091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1056,7 +1108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1073,7 +1125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1090,7 +1142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1107,7 +1159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1124,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1141,7 +1193,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1158,7 +1210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1175,7 +1227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1192,7 +1244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1209,7 +1261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1226,7 +1278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1243,7 +1295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1260,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1277,7 +1329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1294,7 +1346,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1311,7 +1363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1328,7 +1380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1345,7 +1397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1362,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1373,13 +1425,13 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1390,13 +1442,13 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1413,111 +1465,111 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
         <v>1001</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>1001</v>
-      </c>
-      <c r="B33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>1001</v>
-      </c>
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>1001</v>
-      </c>
-      <c r="B35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1001</v>
-      </c>
-      <c r="B36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1001</v>
-      </c>
-      <c r="B37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>1002</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
@@ -1532,9 +1584,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -1549,9 +1601,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
@@ -1566,9 +1618,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B41" t="s">
         <v>17</v>
@@ -1583,9 +1635,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B42" t="s">
         <v>18</v>
@@ -1600,9 +1652,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -1617,15 +1669,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B44" t="s">
         <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
@@ -1634,9 +1686,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
@@ -1651,9 +1703,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>
@@ -1668,9 +1720,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
@@ -1685,9 +1737,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
@@ -1702,9 +1754,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
@@ -1716,6 +1768,108 @@
         <v>4</v>
       </c>
       <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>1003</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>1003</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>1003</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>1003</v>
+      </c>
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>1003</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>1003</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1732,12 +1886,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1745,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1753,7 +1907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1761,7 +1915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1769,7 +1923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1777,7 +1931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1785,7 +1939,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1793,7 +1947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1801,12 +1955,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1816,18 +1970,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1835,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1843,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1851,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1859,7 +2013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1867,7 +2021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1875,7 +2029,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1883,7 +2037,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1891,7 +2045,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1899,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1907,7 +2061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1915,7 +2069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1923,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1931,7 +2085,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1939,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1947,7 +2101,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1955,7 +2109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1963,7 +2117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1971,7 +2125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1979,7 +2133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1987,7 +2141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1995,12 +2149,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22">
         <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2016,13 +2186,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2030,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2038,7 +2208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2046,7 +2216,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2054,7 +2224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2062,7 +2232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2070,7 +2240,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
changes to experiment template
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA148A1-34AB-F24F-A7FC-0B7CCA1B3AF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11600467-A533-B74A-B4E0-32F10FE20316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -236,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -587,14 +587,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="83.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +614,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -634,7 +634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -654,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -674,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -694,7 +694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -734,7 +734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -774,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1">
+    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -794,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1">
+    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -814,7 +814,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17" customHeight="1">
+    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -834,7 +834,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" customHeight="1">
+    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -854,7 +854,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1001</v>
       </c>
@@ -874,7 +874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1002</v>
       </c>
@@ -894,7 +894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1003</v>
       </c>
@@ -923,11 +923,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
@@ -938,7 +938,7 @@
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -972,7 +972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -989,7 +989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1425,13 +1425,13 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
         <v>57</v>
       </c>
-      <c r="E29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1442,13 +1442,13 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
         <v>57</v>
       </c>
-      <c r="E30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1476,13 +1476,13 @@
         <v>65</v>
       </c>
       <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
         <v>57</v>
       </c>
-      <c r="E32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>11</v>
       </c>
@@ -1493,13 +1493,13 @@
         <v>65</v>
       </c>
       <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
         <v>57</v>
       </c>
-      <c r="E33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>11</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>12</v>
       </c>
@@ -1527,13 +1527,13 @@
         <v>65</v>
       </c>
       <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
         <v>57</v>
       </c>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1544,13 +1544,13 @@
         <v>65</v>
       </c>
       <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
         <v>57</v>
       </c>
-      <c r="E36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1001</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1001</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1001</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1001</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1001</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1001</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1002</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1002</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1002</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1002</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1002</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1002</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1003</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1003</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1003</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1003</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1003</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1003</v>
       </c>
@@ -1886,12 +1886,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1972,16 +1972,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -2186,13 +2186,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added support for labels
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11600467-A533-B74A-B4E0-32F10FE20316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BB8D5E-E1A3-EB49-A41B-26CEE8E1030C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="81">
   <si>
     <t>experiment_id</t>
   </si>
@@ -230,6 +230,48 @@
   </si>
   <si>
     <t>Compare Ferguson models</t>
+  </si>
+  <si>
+    <t>Compare base and best with Ferguson</t>
+  </si>
+  <si>
+    <t>Ferguson Iceland age-simple</t>
+  </si>
+  <si>
+    <t>Compare Ferguson Iceland models</t>
+  </si>
+  <si>
+    <t>label_english</t>
+  </si>
+  <si>
+    <t>label_icelandic</t>
+  </si>
+  <si>
+    <t>Base model</t>
+  </si>
+  <si>
+    <t>Grunnlíkan</t>
+  </si>
+  <si>
+    <t>Bætt líkan</t>
+  </si>
+  <si>
+    <t>Improved model</t>
+  </si>
+  <si>
+    <t>Ferguson Wuhan</t>
+  </si>
+  <si>
+    <t>Ferguson Iceland</t>
+  </si>
+  <si>
+    <t>CA model</t>
+  </si>
+  <si>
+    <t>KM grunnlíkan</t>
+  </si>
+  <si>
+    <t>Ferguson Ísland</t>
   </si>
 </sst>
 </file>
@@ -581,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,7 +636,7 @@
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,8 +655,14 @@
       <c r="F1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -633,8 +681,14 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -654,7 +708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -674,7 +728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -693,8 +747,14 @@
       <c r="F5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -714,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -734,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -754,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -774,7 +834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -794,7 +854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -813,8 +873,14 @@
       <c r="F11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -833,8 +899,14 @@
       <c r="F12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -854,38 +926,38 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>1001</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1002</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -893,13 +965,19 @@
       <c r="F15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -911,6 +989,26 @@
         <v>6</v>
       </c>
       <c r="F16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1003</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -921,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:D36"/>
+    <sheetView topLeftCell="A15" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1569,16 +1667,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1001</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
         <v>4</v>
@@ -1586,16 +1684,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>1001</v>
+        <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E39" t="s">
         <v>4</v>
@@ -1603,16 +1701,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>1001</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E40" t="s">
         <v>6</v>
@@ -1623,7 +1721,7 @@
         <v>1001</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -1632,7 +1730,7 @@
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1640,7 +1738,7 @@
         <v>1001</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -1649,7 +1747,7 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1657,7 +1755,7 @@
         <v>1001</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -1671,10 +1769,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -1683,15 +1781,15 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -1700,15 +1798,15 @@
         <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -1725,7 +1823,7 @@
         <v>1002</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
@@ -1734,7 +1832,7 @@
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1742,7 +1840,7 @@
         <v>1002</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
@@ -1751,7 +1849,7 @@
         <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1759,7 +1857,7 @@
         <v>1002</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
@@ -1773,27 +1871,27 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
@@ -1802,15 +1900,15 @@
         <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
@@ -1827,16 +1925,16 @@
         <v>1003</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
       </c>
       <c r="E53" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1844,7 +1942,7 @@
         <v>1003</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -1853,7 +1951,7 @@
         <v>4</v>
       </c>
       <c r="E54" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1861,15 +1959,66 @@
         <v>1003</v>
       </c>
       <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1003</v>
+      </c>
+      <c r="B56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1003</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1003</v>
+      </c>
+      <c r="B58" t="s">
         <v>19</v>
       </c>
-      <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1880,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1963,6 +2112,22 @@
         <v>66</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1970,10 +2135,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2171,6 +2336,54 @@
       </c>
       <c r="B24">
         <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added experiments and runs
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BB8D5E-E1A3-EB49-A41B-26CEE8E1030C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D06BC9-E147-0B4B-ADDE-CCC9123C9117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="980" windowWidth="25600" windowHeight="14720" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="89">
   <si>
     <t>experiment_id</t>
   </si>
@@ -272,6 +272,30 @@
   </si>
   <si>
     <t>Ferguson Ísland</t>
+  </si>
+  <si>
+    <t>Compare Base and Best</t>
+  </si>
+  <si>
+    <t>Compare Base and CA base</t>
+  </si>
+  <si>
+    <t>Compare Best and Ferguson Iceland</t>
+  </si>
+  <si>
+    <t>Base age_official</t>
+  </si>
+  <si>
+    <t>LOS driven: 4+age_official</t>
+  </si>
+  <si>
+    <t>Base: age_simple and age_official</t>
+  </si>
+  <si>
+    <t>Best: age_simple and age_official</t>
+  </si>
+  <si>
+    <t>age_official_point_of_diagnosis</t>
   </si>
 </sst>
 </file>
@@ -623,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,15 +970,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1001</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
         <v>31</v>
@@ -965,22 +989,16 @@
       <c r="F15" t="s">
         <v>6</v>
       </c>
-      <c r="G15" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1002</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -992,23 +1010,69 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1002</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
         <v>32</v>
       </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1003</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1019,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A31" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,50 +1782,50 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>1001</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1001</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>1001</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
         <v>6</v>
@@ -1769,33 +1833,33 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>1001</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E44" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>1001</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
         <v>6</v>
@@ -1803,16 +1867,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>1001</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E46" t="s">
         <v>6</v>
@@ -1820,7 +1884,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B47" t="s">
         <v>14</v>
@@ -1837,7 +1901,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B48" t="s">
         <v>15</v>
@@ -1854,7 +1918,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -1871,7 +1935,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -1888,7 +1952,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
@@ -1905,7 +1969,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
@@ -1922,13 +1986,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B53" t="s">
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
@@ -1939,7 +2003,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B54" t="s">
         <v>15</v>
@@ -1956,7 +2020,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B55" t="s">
         <v>16</v>
@@ -1973,7 +2037,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B56" t="s">
         <v>17</v>
@@ -1990,7 +2054,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
@@ -2007,7 +2071,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
@@ -2019,6 +2083,108 @@
         <v>4</v>
       </c>
       <c r="E58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1003</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1003</v>
+      </c>
+      <c r="B60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1003</v>
+      </c>
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1003</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1003</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1003</v>
+      </c>
+      <c r="B64" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2029,10 +2195,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2128,6 +2294,46 @@
         <v>69</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2135,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2332,10 +2538,10 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2343,7 +2549,7 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2351,7 +2557,7 @@
         <v>9</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2359,12 +2565,12 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>11</v>
@@ -2375,15 +2581,87 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>13</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gagnabord test adding files
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Signy/Projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D981D5-88F1-2B4D-AE23-9C9B4DEC4FA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A913073A-6FB2-9646-9B1D-44E5FCCD38E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1320" yWindow="-17000" windowWidth="25600" windowHeight="14260" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="run_specification" sheetId="3" r:id="rId4"/>
     <sheet name="heuristics_description" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="107">
   <si>
     <t>experiment_id</t>
   </si>
@@ -299,13 +299,64 @@
   </si>
   <si>
     <t>KM grunnlíkan</t>
+  </si>
+  <si>
+    <t>nytt</t>
+  </si>
+  <si>
+    <t>nytt prufa</t>
+  </si>
+  <si>
+    <t>base model with date_first_symptoms instead of date_diagnosis</t>
+  </si>
+  <si>
+    <t>symptoms</t>
+  </si>
+  <si>
+    <t>Date of first symptoms</t>
+  </si>
+  <si>
+    <t>Dagseting fyrstu einkenna</t>
+  </si>
+  <si>
+    <t>date_symptoms</t>
+  </si>
+  <si>
+    <t>LOS driven: 3 + age-point of diag splitting of transitions in Inpatient Ward, first_symptoms</t>
+  </si>
+  <si>
+    <t>symptoms improved</t>
+  </si>
+  <si>
+    <t>bætt líkan með symptoms</t>
+  </si>
+  <si>
+    <t>4 með date_symptoms</t>
+  </si>
+  <si>
+    <t>Transition driven: 1 + hospital_less_than_14_days heuristic,first_symptoms</t>
+  </si>
+  <si>
+    <t>LOS driven:3 + treatment constraints splitting of transitions  in Inpatient Ward,first_symptoms</t>
+  </si>
+  <si>
+    <t>6 with date_symptoms</t>
+  </si>
+  <si>
+    <t>7 with date_symptoms</t>
+  </si>
+  <si>
+    <t>Only improved model</t>
+  </si>
+  <si>
+    <t>Only ferguson wuhan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -649,21 +700,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="83.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +740,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -715,7 +766,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -735,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -755,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -781,7 +832,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -801,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -821,7 +872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -841,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -861,7 +912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" customHeight="1">
+    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -881,7 +932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" customHeight="1">
+    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -907,7 +958,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" customHeight="1">
+    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -933,7 +984,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" customHeight="1">
+    <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -953,7 +1004,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17" customHeight="1">
+    <row r="14" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -973,7 +1024,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17" customHeight="1">
+    <row r="15" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -993,7 +1044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" customHeight="1">
+    <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1013,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1001</v>
       </c>
@@ -1039,7 +1090,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1002</v>
       </c>
@@ -1059,7 +1110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1003</v>
       </c>
@@ -1077,6 +1128,130 @@
       </c>
       <c r="F19" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2001</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2004</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2006</v>
+      </c>
+      <c r="B23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2007</v>
+      </c>
+      <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1085,14 +1260,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
-  <dimension ref="A1:E64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A50" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:E82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
@@ -1103,7 +1278,7 @@
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1137,7 +1312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1154,7 +1329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1171,7 +1346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1188,7 +1363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1205,7 +1380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1222,7 +1397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1239,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1256,7 +1431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1273,7 +1448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1290,7 +1465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1307,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1324,7 +1499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1341,7 +1516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1358,7 +1533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1375,7 +1550,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1392,7 +1567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1409,7 +1584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1426,7 +1601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1443,7 +1618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1460,7 +1635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1477,7 +1652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1494,7 +1669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1511,7 +1686,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1528,7 +1703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1545,7 +1720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1562,7 +1737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1579,7 +1754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1596,7 +1771,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1613,7 +1788,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1630,7 +1805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1647,7 +1822,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>11</v>
       </c>
@@ -1664,7 +1839,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>11</v>
       </c>
@@ -1681,7 +1856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>12</v>
       </c>
@@ -1698,7 +1873,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1715,7 +1890,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1732,7 +1907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>13</v>
       </c>
@@ -1749,7 +1924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>13</v>
       </c>
@@ -1766,7 +1941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>13</v>
       </c>
@@ -1783,7 +1958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1800,7 +1975,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>14</v>
       </c>
@@ -1817,7 +1992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>14</v>
       </c>
@@ -1834,7 +2009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>15</v>
       </c>
@@ -1851,7 +2026,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>15</v>
       </c>
@@ -1868,7 +2043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>15</v>
       </c>
@@ -1885,7 +2060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1001</v>
       </c>
@@ -1902,7 +2077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1001</v>
       </c>
@@ -1919,7 +2094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1001</v>
       </c>
@@ -1936,7 +2111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1001</v>
       </c>
@@ -1953,7 +2128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1001</v>
       </c>
@@ -1970,7 +2145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1001</v>
       </c>
@@ -1987,7 +2162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1002</v>
       </c>
@@ -2004,7 +2179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1002</v>
       </c>
@@ -2021,7 +2196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1002</v>
       </c>
@@ -2038,7 +2213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1002</v>
       </c>
@@ -2055,7 +2230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1002</v>
       </c>
@@ -2072,7 +2247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1002</v>
       </c>
@@ -2089,7 +2264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1003</v>
       </c>
@@ -2106,7 +2281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1003</v>
       </c>
@@ -2123,7 +2298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1003</v>
       </c>
@@ -2140,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1003</v>
       </c>
@@ -2157,7 +2332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1003</v>
       </c>
@@ -2174,7 +2349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1003</v>
       </c>
@@ -2188,6 +2363,261 @@
         <v>4</v>
       </c>
       <c r="E64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2001</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2001</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2001</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2004</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2004</v>
+      </c>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2004</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2006</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2006</v>
+      </c>
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2006</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2007</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2007</v>
+      </c>
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2007</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2197,19 +2627,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B16"/>
+      <selection activeCell="A24" sqref="A24:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2217,7 +2647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2225,7 +2655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2233,7 +2663,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2241,7 +2671,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2249,7 +2679,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2257,7 +2687,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2265,7 +2695,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2273,7 +2703,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2281,7 +2711,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2289,7 +2719,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2297,7 +2727,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2305,7 +2735,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2313,7 +2743,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2321,7 +2751,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2329,12 +2759,68 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2001</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2004</v>
+      </c>
+      <c r="B19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2343,19 +2829,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
-  <dimension ref="A1:B40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:I17"/>
+    <sheetView topLeftCell="A39" zoomScale="120" workbookViewId="0">
+      <selection activeCell="B49" sqref="A49:B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2363,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2371,7 +2857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2379,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2387,7 +2873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2395,7 +2881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2403,7 +2889,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2411,7 +2897,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2419,7 +2905,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2427,7 +2913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2435,7 +2921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2443,7 +2929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2451,7 +2937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -2459,7 +2945,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2467,7 +2953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -2475,7 +2961,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2483,7 +2969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2491,7 +2977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -2499,7 +2985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7</v>
       </c>
@@ -2507,7 +2993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -2515,7 +3001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -2523,7 +3009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
@@ -2531,7 +3017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -2539,7 +3025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -2547,7 +3033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>9</v>
       </c>
@@ -2555,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2563,7 +3049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2571,7 +3057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -2579,7 +3065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -2587,7 +3073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -2595,7 +3081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11</v>
       </c>
@@ -2603,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>11</v>
       </c>
@@ -2611,7 +3097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>12</v>
       </c>
@@ -2619,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>12</v>
       </c>
@@ -2627,7 +3113,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>13</v>
       </c>
@@ -2635,7 +3121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>13</v>
       </c>
@@ -2643,7 +3129,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>14</v>
       </c>
@@ -2651,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>14</v>
       </c>
@@ -2659,7 +3145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>15</v>
       </c>
@@ -2667,12 +3153,76 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>15</v>
       </c>
       <c r="B40">
         <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>16</v>
+      </c>
+      <c r="B41">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2001</v>
+      </c>
+      <c r="B42">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2004</v>
+      </c>
+      <c r="B43">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2006</v>
+      </c>
+      <c r="B44">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2006</v>
+      </c>
+      <c r="B45">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2007</v>
+      </c>
+      <c r="B46">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2681,20 +3231,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16803A79-36E8-C242-9A3E-7A10F403054B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2702,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2710,7 +3260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2718,7 +3268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2726,7 +3276,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2734,7 +3284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2742,7 +3292,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
adding vaccine to simulation
</commit_message>
<xml_diff>
--- a/lsh_data_processing/experiment_template.xlsx
+++ b/lsh_data_processing/experiment_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Signy/Projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magga Vala\Documents\vinna\BCS\lsh_data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A913073A-6FB2-9646-9B1D-44E5FCCD38E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="28800" windowHeight="17538" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_description" sheetId="2" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="115">
   <si>
     <t>experiment_id</t>
   </si>
@@ -350,12 +349,36 @@
   </si>
   <si>
     <t>Only ferguson wuhan</t>
+  </si>
+  <si>
+    <t>prufa</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>age_simple_vaccinated</t>
+  </si>
+  <si>
+    <t>19, but time_dependent splitting 10 days</t>
+  </si>
+  <si>
+    <t>ten days</t>
+  </si>
+  <si>
+    <t>10 days</t>
+  </si>
+  <si>
+    <t>10 daga split</t>
+  </si>
+  <si>
+    <t>length_of_stay_simple_ten_days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -700,21 +723,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="C22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="83.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.84765625" customWidth="1"/>
+    <col min="2" max="2" width="83.34765625" customWidth="1"/>
+    <col min="5" max="5" width="13.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,7 +763,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -766,7 +789,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -786,7 +809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -806,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -832,7 +855,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -852,7 +875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -872,7 +895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -892,7 +915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -912,7 +935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="17.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -932,7 +955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="17.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -958,7 +981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="17.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -984,7 +1007,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="17.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1004,7 +1027,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="17.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1024,7 +1047,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="17.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1044,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="17.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1064,7 +1087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A17">
         <v>1001</v>
       </c>
@@ -1090,7 +1113,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A18">
         <v>1002</v>
       </c>
@@ -1110,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A19">
         <v>1003</v>
       </c>
@@ -1130,7 +1153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1150,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A21">
         <v>2001</v>
       </c>
@@ -1176,7 +1199,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -1202,7 +1225,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A23">
         <v>2006</v>
       </c>
@@ -1228,7 +1251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A24">
         <v>2007</v>
       </c>
@@ -1252,6 +1275,58 @@
       </c>
       <c r="H24">
         <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1260,25 +1335,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:E82"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="5" width="38.1640625" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.84765625" customWidth="1"/>
+    <col min="2" max="2" width="22.6484375" customWidth="1"/>
+    <col min="3" max="3" width="32.1484375" customWidth="1"/>
+    <col min="4" max="5" width="38.1484375" customWidth="1"/>
+    <col min="6" max="6" width="31.1484375" customWidth="1"/>
+    <col min="7" max="7" width="13.84765625" customWidth="1"/>
+    <col min="8" max="8" width="18.84765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1295,7 +1370,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1312,7 +1387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1329,7 +1404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1346,7 +1421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1363,7 +1438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1380,7 +1455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1397,7 +1472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1414,7 +1489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1431,7 +1506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1448,7 +1523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1465,7 +1540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1482,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1499,7 +1574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1516,7 +1591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1533,7 +1608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1550,7 +1625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1567,7 +1642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1584,7 +1659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1601,7 +1676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1618,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1635,7 +1710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1652,7 +1727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1669,7 +1744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1686,7 +1761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1703,7 +1778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1720,7 +1795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1737,7 +1812,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1754,7 +1829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1771,7 +1846,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1788,7 +1863,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1805,7 +1880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1822,7 +1897,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A33">
         <v>11</v>
       </c>
@@ -1839,7 +1914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A34">
         <v>11</v>
       </c>
@@ -1856,7 +1931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A35">
         <v>12</v>
       </c>
@@ -1873,7 +1948,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1890,7 +1965,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1907,7 +1982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A38">
         <v>13</v>
       </c>
@@ -1924,7 +1999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A39">
         <v>13</v>
       </c>
@@ -1941,7 +2016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A40">
         <v>13</v>
       </c>
@@ -1958,7 +2033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1975,7 +2050,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A42">
         <v>14</v>
       </c>
@@ -1992,7 +2067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A43">
         <v>14</v>
       </c>
@@ -2009,7 +2084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A44">
         <v>15</v>
       </c>
@@ -2026,7 +2101,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A45">
         <v>15</v>
       </c>
@@ -2043,7 +2118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A46">
         <v>15</v>
       </c>
@@ -2060,7 +2135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A47">
         <v>1001</v>
       </c>
@@ -2077,7 +2152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A48">
         <v>1001</v>
       </c>
@@ -2094,7 +2169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A49">
         <v>1001</v>
       </c>
@@ -2111,7 +2186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A50">
         <v>1001</v>
       </c>
@@ -2128,7 +2203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A51">
         <v>1001</v>
       </c>
@@ -2145,7 +2220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A52">
         <v>1001</v>
       </c>
@@ -2162,7 +2237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A53">
         <v>1002</v>
       </c>
@@ -2179,7 +2254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A54">
         <v>1002</v>
       </c>
@@ -2196,7 +2271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A55">
         <v>1002</v>
       </c>
@@ -2213,7 +2288,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A56">
         <v>1002</v>
       </c>
@@ -2230,7 +2305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A57">
         <v>1002</v>
       </c>
@@ -2247,7 +2322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A58">
         <v>1002</v>
       </c>
@@ -2264,7 +2339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A59">
         <v>1003</v>
       </c>
@@ -2281,7 +2356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A60">
         <v>1003</v>
       </c>
@@ -2298,7 +2373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A61">
         <v>1003</v>
       </c>
@@ -2315,7 +2390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A62">
         <v>1003</v>
       </c>
@@ -2332,7 +2407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A63">
         <v>1003</v>
       </c>
@@ -2349,7 +2424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A64">
         <v>1003</v>
       </c>
@@ -2366,7 +2441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A65">
         <v>16</v>
       </c>
@@ -2383,7 +2458,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A66">
         <v>16</v>
       </c>
@@ -2400,7 +2475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A67">
         <v>16</v>
       </c>
@@ -2417,7 +2492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A68">
         <v>2001</v>
       </c>
@@ -2434,7 +2509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A69">
         <v>2001</v>
       </c>
@@ -2451,7 +2526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A70">
         <v>2001</v>
       </c>
@@ -2468,7 +2543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A71">
         <v>2004</v>
       </c>
@@ -2485,7 +2560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A72">
         <v>2004</v>
       </c>
@@ -2502,7 +2577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A73">
         <v>2004</v>
       </c>
@@ -2519,7 +2594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A74">
         <v>2006</v>
       </c>
@@ -2536,7 +2611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A75">
         <v>2006</v>
       </c>
@@ -2553,7 +2628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A76">
         <v>2006</v>
       </c>
@@ -2570,7 +2645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A77">
         <v>2007</v>
       </c>
@@ -2587,7 +2662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A78">
         <v>2007</v>
       </c>
@@ -2604,7 +2679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A79">
         <v>2007</v>
       </c>
@@ -2618,6 +2693,108 @@
         <v>4</v>
       </c>
       <c r="E79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A80">
+        <v>17</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" t="s">
+        <v>109</v>
+      </c>
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A81">
+        <v>17</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>109</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A82">
+        <v>17</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A83">
+        <v>18</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" t="s">
+        <v>109</v>
+      </c>
+      <c r="E83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A84">
+        <v>18</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" t="s">
+        <v>109</v>
+      </c>
+      <c r="E84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A85">
+        <v>18</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2627,19 +2804,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="65.6640625" customWidth="1"/>
+    <col min="2" max="2" width="65.6484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2647,7 +2824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2655,7 +2832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2663,7 +2840,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2671,7 +2848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2679,7 +2856,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2687,7 +2864,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2695,7 +2872,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2703,7 +2880,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2711,7 +2888,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2719,7 +2896,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2727,7 +2904,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2735,7 +2912,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2743,7 +2920,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2751,7 +2928,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2759,7 +2936,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2767,7 +2944,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2775,7 +2952,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A18">
         <v>2001</v>
       </c>
@@ -2783,7 +2960,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A19">
         <v>2004</v>
       </c>
@@ -2791,7 +2968,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>6</v>
       </c>
@@ -2799,7 +2976,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A21">
         <v>7</v>
       </c>
@@ -2807,7 +2984,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A22">
         <v>17</v>
       </c>
@@ -2815,12 +2992,28 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2829,19 +3022,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="120" workbookViewId="0">
-      <selection activeCell="B49" sqref="A49:B49"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.34765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2849,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2857,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2865,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2873,7 +3066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2881,7 +3074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2889,7 +3082,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2897,7 +3090,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2905,7 +3098,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2913,7 +3106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2921,7 +3114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2929,7 +3122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2937,7 +3130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A13">
         <v>5</v>
       </c>
@@ -2945,7 +3138,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2953,7 +3146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A15">
         <v>5</v>
       </c>
@@ -2961,7 +3154,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2969,7 +3162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2977,7 +3170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A18">
         <v>7</v>
       </c>
@@ -2985,7 +3178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A19">
         <v>7</v>
       </c>
@@ -2993,7 +3186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>7</v>
       </c>
@@ -3001,7 +3194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A21">
         <v>7</v>
       </c>
@@ -3009,7 +3202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A22">
         <v>8</v>
       </c>
@@ -3017,7 +3210,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A23">
         <v>8</v>
       </c>
@@ -3025,7 +3218,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A24">
         <v>8</v>
       </c>
@@ -3033,7 +3226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A25">
         <v>9</v>
       </c>
@@ -3041,7 +3234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A26">
         <v>9</v>
       </c>
@@ -3049,7 +3242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A27">
         <v>9</v>
       </c>
@@ -3057,7 +3250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A28">
         <v>9</v>
       </c>
@@ -3065,7 +3258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A29">
         <v>10</v>
       </c>
@@ -3073,7 +3266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A30">
         <v>10</v>
       </c>
@@ -3081,7 +3274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A31">
         <v>11</v>
       </c>
@@ -3089,7 +3282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A32">
         <v>11</v>
       </c>
@@ -3097,7 +3290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A33">
         <v>12</v>
       </c>
@@ -3105,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A34">
         <v>12</v>
       </c>
@@ -3113,7 +3306,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A35">
         <v>13</v>
       </c>
@@ -3121,7 +3314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A36">
         <v>13</v>
       </c>
@@ -3129,7 +3322,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A37">
         <v>14</v>
       </c>
@@ -3137,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A38">
         <v>14</v>
       </c>
@@ -3145,7 +3338,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A39">
         <v>15</v>
       </c>
@@ -3153,7 +3346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A40">
         <v>15</v>
       </c>
@@ -3161,7 +3354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A41">
         <v>16</v>
       </c>
@@ -3169,7 +3362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A42">
         <v>2001</v>
       </c>
@@ -3177,7 +3370,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A43">
         <v>2004</v>
       </c>
@@ -3185,7 +3378,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A44">
         <v>2006</v>
       </c>
@@ -3193,7 +3386,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A45">
         <v>2006</v>
       </c>
@@ -3201,7 +3394,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A46">
         <v>2007</v>
       </c>
@@ -3209,7 +3402,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A47">
         <v>17</v>
       </c>
@@ -3217,12 +3410,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A48">
         <v>18</v>
       </c>
       <c r="B48">
         <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A49">
+        <v>19</v>
+      </c>
+      <c r="B49">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -3231,20 +3440,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="77.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.84765625" customWidth="1"/>
+    <col min="2" max="2" width="77.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3252,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3260,7 +3469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3268,7 +3477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3276,7 +3485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3284,7 +3493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3292,7 +3501,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>